<commit_message>
Auto-committed on 2022/03/18 週五
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L9-報表作業/YearlyHouseLoanInt.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L9-報表作業/YearlyHouseLoanInt.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L9-報表作業\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SKL\DB\GenTables\L9-報表作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51566579-57E5-4E43-9EFC-57975B8805EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29747DED-E9B1-4FF1-B62F-BFB89CFF2341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
     <sheet name="DBS" sheetId="2" r:id="rId2"/>
     <sheet name="SP" sheetId="3" r:id="rId3"/>
+    <sheet name="JsonField" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="84">
   <si>
     <t>SEQ</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -330,6 +331,16 @@
 7:定存特約
 8:劃撥存款</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>DECIMAL</t>
+  </si>
+  <si>
+    <t>bdlocation</t>
+  </si>
+  <si>
+    <t>地址</t>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -579,7 +590,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -711,6 +722,12 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1072,7 +1089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -1088,10 +1105,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="45"/>
+      <c r="B1" s="47"/>
       <c r="C1" s="3" t="s">
         <v>46</v>
       </c>
@@ -1103,8 +1120,8 @@
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="44"/>
-      <c r="B2" s="45"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="47"/>
       <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
@@ -1116,10 +1133,10 @@
       <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="47"/>
+      <c r="B3" s="49"/>
       <c r="C3" s="11" t="s">
         <v>63</v>
       </c>
@@ -1131,20 +1148,20 @@
       <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="46"/>
+      <c r="B4" s="48"/>
       <c r="D4" s="12"/>
       <c r="E4" s="9"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="47"/>
+      <c r="B5" s="49"/>
       <c r="C5" s="11"/>
       <c r="D5" s="12"/>
       <c r="E5" s="9"/>
@@ -1152,10 +1169,10 @@
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="45"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="11"/>
       <c r="D6" s="12"/>
       <c r="E6" s="9"/>
@@ -1163,10 +1180,10 @@
       <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="46"/>
+      <c r="B7" s="48"/>
       <c r="C7" s="3"/>
       <c r="D7" s="12"/>
       <c r="E7" s="9"/>
@@ -1662,4 +1679,57 @@
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5602C9A7-B2E5-41B8-872A-8B4873F54873}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="45">
+        <v>1</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="45"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="45"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="15" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>